<commit_message>
learing excel read and write in R
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -6,18 +6,27 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="City" r:id="rId3" sheetId="1"/>
+    <sheet name="Seconde Sheet" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>X....city</t>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>dept</t>
   </si>
   <si>
     <t>1</t>
@@ -47,53 +56,46 @@
     <t>Rick</t>
   </si>
   <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michelle  </t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>Gary</t>
+    <t xml:space="preserve">Dan </t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gary </t>
   </si>
   <si>
     <t>Nina</t>
   </si>
   <si>
-    <t>Simon</t>
+    <t xml:space="preserve">Simon </t>
   </si>
   <si>
     <t>Guru</t>
   </si>
   <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>Tampa</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>Dallas</t>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Finance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -123,8 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -145,92 +149,173 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D2" t="n">
+        <v>623.3</v>
+      </c>
+      <c r="E2" t="n" s="2">
+        <v>40909.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="D3" t="n">
+        <v>515.2</v>
+      </c>
+      <c r="E3" t="n" s="2">
+        <v>41540.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.0</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>611.0</v>
+      </c>
+      <c r="E4" t="n" s="2">
+        <v>41958.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.0</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="D5" t="n">
+        <v>729.0</v>
+      </c>
+      <c r="E5" t="n" s="2">
+        <v>41770.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="E6" t="n" s="2">
+        <v>42090.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="D7" t="n">
+        <v>578.0</v>
+      </c>
+      <c r="E7" t="n" s="2">
+        <v>41415.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D8" t="n">
+        <v>632.8</v>
+      </c>
+      <c r="E8" t="n" s="2">
+        <v>41485.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8.0</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="n">
+        <v>722.5</v>
+      </c>
+      <c r="E9" t="n" s="2">
+        <v>41807.0</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>